<commit_message>
feat: add duplicate key check to batch upload and added more cohort data examples
</commit_message>
<xml_diff>
--- a/data/datacatalogue/Cohorts.xlsx
+++ b/data/datacatalogue/Cohorts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/data/datacatalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEF00E1-DCD6-0D48-9167-16F16DAA6EFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8751C95-1A25-7D46-A9AF-5F0C481571A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="21" activeTab="30" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="Institutions" sheetId="20" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11842" uniqueCount="3905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11878" uniqueCount="3945">
   <si>
     <t>name</t>
   </si>
@@ -11846,6 +11846,126 @@
   </si>
   <si>
     <t>Raineadmin</t>
+  </si>
+  <si>
+    <t>EUChildNetwork</t>
+  </si>
+  <si>
+    <t>The Network</t>
+  </si>
+  <si>
+    <t>square_meter_per_square_kilometer</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>square_meter</t>
+  </si>
+  <si>
+    <t>meter_per_square_kilometer</t>
+  </si>
+  <si>
+    <t>percent_energy_intake</t>
+  </si>
+  <si>
+    <t>inverse_meter</t>
+  </si>
+  <si>
+    <t>hours_per_day</t>
+  </si>
+  <si>
+    <t>A_weighted_decibel</t>
+  </si>
+  <si>
+    <t>gram_per_dl</t>
+  </si>
+  <si>
+    <t>percent_total_food</t>
+  </si>
+  <si>
+    <t>ng_per_ml</t>
+  </si>
+  <si>
+    <t>dogs</t>
+  </si>
+  <si>
+    <t>Kcal_per_day</t>
+  </si>
+  <si>
+    <t>mg_per_dl</t>
+  </si>
+  <si>
+    <t>vehicles_per_day</t>
+  </si>
+  <si>
+    <t>ten_power_minus_five_per_inverse_meter</t>
+  </si>
+  <si>
+    <t>parts_per_billion</t>
+  </si>
+  <si>
+    <t>vehicles_per_day_and_meter</t>
+  </si>
+  <si>
+    <t>iu_per_ml</t>
+  </si>
+  <si>
+    <t>milligram_per_day</t>
+  </si>
+  <si>
+    <t>nanograms_per_cubic_meter</t>
+  </si>
+  <si>
+    <t>people_per_square_kilometer</t>
+  </si>
+  <si>
+    <t>gram_per_day</t>
+  </si>
+  <si>
+    <t>micrograms_per_cubic_meter</t>
+  </si>
+  <si>
+    <t>ndvi_value</t>
+  </si>
+  <si>
+    <t>sympercent_change</t>
+  </si>
+  <si>
+    <t>number_per_square_kilometer</t>
+  </si>
+  <si>
+    <t>µg/ml</t>
+  </si>
+  <si>
+    <t>servings_per_day</t>
+  </si>
+  <si>
+    <t>kilojoules_per_square_meter</t>
+  </si>
+  <si>
+    <t>gram/ml</t>
+  </si>
+  <si>
+    <t>times_per_day</t>
+  </si>
+  <si>
+    <t>cats</t>
+  </si>
+  <si>
+    <t>degree_celsius</t>
+  </si>
+  <si>
+    <t>z-score</t>
+  </si>
+  <si>
+    <t>kua_l</t>
+  </si>
+  <si>
+    <t>times_per_week</t>
   </si>
 </sst>
 </file>
@@ -13438,14 +13558,14 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48C5E39-1D29-754B-A3C5-D51551FFE247}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D10" sqref="D10"/>
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
-      <selection pane="bottomRight" activeCell="C196" sqref="C21:C196"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13552,6 +13672,17 @@
       </c>
       <c r="C6" s="5" t="s">
         <v>278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>3905</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -51687,10 +51818,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DE7E7C-E4DA-A54C-8D3C-754EAD159BE9}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -51851,6 +51982,196 @@
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>540</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>3907</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>3908</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>3909</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>3910</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>3911</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>3912</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>3913</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>3914</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>3915</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>3916</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>3917</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>3918</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>3919</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>3920</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>3921</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>3922</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>3923</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>3924</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>3925</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>3926</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>3927</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>3929</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>3930</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>3931</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>3932</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>3933</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>3934</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>3935</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>3936</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>3937</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>3938</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>3939</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>3941</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>3942</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>3943</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>3944</v>
       </c>
     </row>
   </sheetData>
@@ -51973,13 +52294,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F669E815-91F3-614D-A79B-23630F6A2A2E}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="37" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -52242,188 +52563,154 @@
     </row>
     <row r="10" spans="1:20" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>3816</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>22</v>
+        <v>3831</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>3858</v>
+        <v>3882</v>
       </c>
       <c r="F10" t="s">
-        <v>184</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3816</v>
+        <v>3817</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>3831</v>
+        <v>3832</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>3882</v>
+        <v>3859</v>
       </c>
       <c r="F11" t="s">
-        <v>3842</v>
+        <v>3846</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>3817</v>
+        <v>3818</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>3832</v>
+        <v>3833</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>3859</v>
+        <v>3860</v>
       </c>
       <c r="F12" t="s">
-        <v>3846</v>
+        <v>3847</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3818</v>
+        <v>3819</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>3833</v>
+        <v>3834</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>3860</v>
+        <v>3861</v>
       </c>
       <c r="F13" t="s">
-        <v>3847</v>
+        <v>3848</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3819</v>
+        <v>3820</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>3834</v>
+        <v>3835</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>3861</v>
+        <v>3862</v>
       </c>
       <c r="F14" t="s">
-        <v>3848</v>
+        <v>3849</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>3820</v>
+        <v>3821</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>3835</v>
+        <v>3836</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>3862</v>
+        <v>3904</v>
       </c>
       <c r="F15" t="s">
-        <v>3849</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>3821</v>
+        <v>3822</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>3836</v>
+        <v>3837</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>3904</v>
+        <v>3863</v>
       </c>
       <c r="F16" t="s">
-        <v>3850</v>
+        <v>3851</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3822</v>
+        <v>3823</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>3837</v>
+        <v>3838</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>3863</v>
+        <v>3864</v>
       </c>
       <c r="F17" t="s">
-        <v>3851</v>
+        <v>3852</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>3823</v>
+        <v>3824</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>3838</v>
+        <v>3839</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>3864</v>
+        <v>3866</v>
       </c>
       <c r="F18" t="s">
-        <v>3852</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>3865</v>
-      </c>
-      <c r="F19" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>3824</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>3839</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
-        <v>3866</v>
-      </c>
-      <c r="F20" t="s">
         <v>3853</v>
       </c>
     </row>
@@ -52473,10 +52760,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A722C4-6F5C-1348-A6B2-F570560B9BB1}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -52584,6 +52871,17 @@
       </c>
       <c r="F4" s="6" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>3905</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>3906</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -52619,10 +52917,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0164DE-D2AE-A246-ABFF-DCD382408FE9}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -52681,6 +52979,14 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3905</v>
+      </c>
+      <c r="B6" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test: adapted Cohorts.xlsx to SampleCategories and DataCategories
</commit_message>
<xml_diff>
--- a/data/datacatalogue/Cohorts.xlsx
+++ b/data/datacatalogue/Cohorts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/data/datacatalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBE3243-13F0-5249-8AFD-6C25F8D0CC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35028941-22D2-C445-B808-7846509A7073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="15" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="3" activeTab="15" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="Institutions" sheetId="20" r:id="rId1"/>
@@ -12315,12 +12315,6 @@
     <t>Age/birthdate,Family and household structure</t>
   </si>
   <si>
-    <t>SampleSources</t>
-  </si>
-  <si>
-    <t>DataSources</t>
-  </si>
-  <si>
     <t>Questionnaires</t>
   </si>
   <si>
@@ -12346,6 +12340,12 @@
   </si>
   <si>
     <t>CollectionTypes</t>
+  </si>
+  <si>
+    <t>SampleCategories</t>
+  </si>
+  <si>
+    <t>DataCategories</t>
   </si>
 </sst>
 </file>
@@ -48111,7 +48111,7 @@
   <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -48956,39 +48956,39 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>4064</v>
+        <v>4073</v>
       </c>
       <c r="B102" t="s">
-        <v>4068</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>4064</v>
+        <v>4073</v>
       </c>
       <c r="B103" t="s">
-        <v>4069</v>
+        <v>4067</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>4065</v>
+        <v>4074</v>
       </c>
       <c r="B104" t="s">
-        <v>4066</v>
+        <v>4064</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
+        <v>4074</v>
+      </c>
+      <c r="B105" t="s">
         <v>4065</v>
-      </c>
-      <c r="B105" t="s">
-        <v>4067</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>4071</v>
+        <v>4069</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>4062</v>
@@ -48996,18 +48996,18 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>4071</v>
+        <v>4069</v>
       </c>
       <c r="B107" t="s">
-        <v>4070</v>
+        <v>4068</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>4074</v>
+        <v>4072</v>
       </c>
       <c r="B108" t="s">
-        <v>4073</v>
+        <v>4071</v>
       </c>
     </row>
   </sheetData>
@@ -49450,7 +49450,7 @@
         <v>4053</v>
       </c>
       <c r="Z1" s="23" t="s">
-        <v>4072</v>
+        <v>4070</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="37" customFormat="1" ht="18" customHeight="1">
@@ -49530,7 +49530,7 @@
         <v>4055</v>
       </c>
       <c r="Z2" s="37" t="s">
-        <v>4073</v>
+        <v>4071</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="37" customHeight="1">
@@ -54617,21 +54617,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006E5135F48701C94A82BE43B430F845A8" ma:contentTypeVersion="6" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="aca3a74f98ee42c448e6b469b1baac44">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="53be7e9d-bfd1-4623-ad00-4bb592644a26" xmlns:ns3="223b7e1d-1c2f-4f50-a58d-c9707aa4074f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ab38790b23a18439c2a0eba974b1b1d" ns2:_="" ns3:_="">
     <xsd:import namespace="53be7e9d-bfd1-4623-ad00-4bb592644a26"/>
@@ -54810,24 +54795,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BCFFD05-1E3E-4C4E-9105-2BD45851CC33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B8B4FE9-00A7-4C89-9DF8-43058C69DC20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA2A984D-D8B4-47A1-94C8-CEB3C0C45FB5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54844,4 +54827,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B8B4FE9-00A7-4C89-9DF8-43058C69DC20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BCFFD05-1E3E-4C4E-9105-2BD45851CC33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>